<commit_message>
Fixing issues with templates
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_sample.xlsx
+++ b/src/assets/empty/faang_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6F1FD9-F105-404A-9482-26B245B7B84B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A8A299-52A3-E549-8C2B-F7293E891633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="2840" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" activeTab="7" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="139">
   <si>
     <t>Sample Name</t>
   </si>
@@ -2023,7 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD35D17F-18C2-864A-BEE4-81B125D47F43}">
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
@@ -2947,169 +2947,249 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9303EA7-3987-8B45-AFF2-6BE5F3BB97EC}">
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="29" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AK1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3122,7 +3202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1503EB05-5C8B-964B-81F7-3D25D9E03BCE}">
   <dimension ref="A1:BW1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Adding modular rules to samples
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_sample.xlsx
+++ b/src/assets/empty/faang_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFB3926-B0A1-1A4C-BAAD-95935AA82832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D1365C-8E53-C84D-8FF6-EFBCF049CF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" activeTab="7" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
   </bookViews>
@@ -454,13 +454,13 @@
     <t>Water Rearing System</t>
   </si>
   <si>
-    <t>Sampling Data Start Time</t>
-  </si>
-  <si>
-    <t>Sampling Data End Time</t>
-  </si>
-  <si>
     <t>Method Of Euthanasia</t>
+  </si>
+  <si>
+    <t>Sampling Day Start Time</t>
+  </si>
+  <si>
+    <t>Sampling Day End Time</t>
   </si>
 </sst>
 </file>
@@ -3202,8 +3202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1503EB05-5C8B-964B-81F7-3D25D9E03BCE}">
   <dimension ref="A1:BW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AY4" sqref="AY4"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BV1" sqref="BV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3498,13 +3498,13 @@
         <v>10</v>
       </c>
       <c r="BT1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BV1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="BW1" s="1" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Updating template with ENA required columns
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_sample.xlsx
+++ b/src/assets/empty/faang_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D1365C-8E53-C84D-8FF6-EFBCF049CF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3AAC49-4DEF-CE4B-B369-D87E6C4B1520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" activeTab="7" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="3" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="141">
   <si>
     <t>Sample Name</t>
   </si>
@@ -461,6 +461,12 @@
   </si>
   <si>
     <t>Sampling Day End Time</t>
+  </si>
+  <si>
+    <t>Collection Date</t>
+  </si>
+  <si>
+    <t>Geographic Location</t>
   </si>
 </sst>
 </file>
@@ -535,25 +541,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,100 +900,99 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="12" t="s">
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="12" t="s">
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="12" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
@@ -1013,83 +1011,82 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,52 +1122,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1221,91 +1218,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="12" t="s">
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1515,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED62F57-0BB2-304A-8E43-F2D039525E7F}">
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,30 +1532,33 @@
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.83203125" customWidth="1"/>
-    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1596,287 +1596,293 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="4"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="4"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="AG3" s="2"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="AI3" s="2"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="4"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="AG4" s="2"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="AI4" s="2"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="4"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="4"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="4"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="5"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="4"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="4"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="4"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="5"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1926,7 +1932,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1938,7 +1944,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -2029,139 +2035,138 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="32.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.6640625" style="7" customWidth="1"/>
-    <col min="34" max="34" width="25.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.6640625" style="7" customWidth="1"/>
-    <col min="36" max="36" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="4.6640625" style="7" customWidth="1"/>
-    <col min="38" max="38" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.6640625" customWidth="1"/>
+    <col min="34" max="34" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.6640625" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.6640625" customWidth="1"/>
+    <col min="38" max="38" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="9" t="s">
+      <c r="V1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="9" t="s">
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="9" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AF1" s="1" t="s">
@@ -2182,763 +2187,763 @@
       <c r="AK1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="8"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="13"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="8"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="8"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="8"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="6"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="6"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="6"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="6"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="6"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="6"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="8"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="6"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="8"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="AL33" s="4"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="6"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="AL33" s="2"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="AL34" s="4"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="6"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="AL34" s="2"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="8"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="AL35" s="4"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="6"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="AL35" s="2"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="8"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="AL36" s="4"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="6"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="AL36" s="2"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="8"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="AL37" s="4"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="6"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="AL37" s="2"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="AL38" s="4"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="AL38" s="2"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="8"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="6"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="8"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="6"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="8"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="6"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="8"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="6"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="8"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="6"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="8"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="6"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="8"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="6"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3018,7 +3023,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3030,7 +3035,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3202,7 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1503EB05-5C8B-964B-81F7-3D25D9E03BCE}">
   <dimension ref="A1:BW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+    <sheetView topLeftCell="BE1" workbookViewId="0">
       <selection activeCell="BV1" sqref="BV1"/>
     </sheetView>
   </sheetViews>
@@ -3287,7 +3292,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3299,7 +3304,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3549,7 +3554,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3561,7 +3566,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">

</xml_diff>

<commit_message>
Fixing issues with organoid templates
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_sample.xlsx
+++ b/src/assets/empty/faang_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB25E55-846F-1848-8FE5-678F24ECAD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212E850D-5ED4-694F-BCAD-92DD670CC820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="7" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
+    <workbookView xWindow="34940" yWindow="2080" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="138">
   <si>
     <t>Sample Name</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Diet</t>
   </si>
   <si>
-    <t xml:space="preserve">Organ Model </t>
-  </si>
-  <si>
     <t>Organ Part Model</t>
   </si>
   <si>
@@ -325,24 +322,15 @@
     <t>Freezing Protocol</t>
   </si>
   <si>
-    <t>Input Aggregate Cell Count</t>
-  </si>
-  <si>
     <t>Organoid Passage Protocol</t>
   </si>
   <si>
-    <t>Organoid Age</t>
-  </si>
-  <si>
     <t>Type Of Organoid Culture</t>
   </si>
   <si>
     <t>Organoid Morphology</t>
   </si>
   <si>
-    <t>Embeddded In Matrigel</t>
-  </si>
-  <si>
     <t>Growth Environment</t>
   </si>
   <si>
@@ -464,6 +452,12 @@
   </si>
   <si>
     <t>Geographic Location</t>
+  </si>
+  <si>
+    <t>Organ Model</t>
+  </si>
+  <si>
+    <t>Organoid Passage</t>
   </si>
 </sst>
 </file>
@@ -473,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -517,6 +511,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -535,10 +545,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,8 +561,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent 4" xfId="1" xr:uid="{7187FD71-EFC8-BA4A-9E08-6C322CD7B0ED}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1858,9 +1872,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE77F75-4E48-3E4D-BF43-36F736F051D4}">
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1872,7 +1888,7 @@
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -1880,110 +1896,102 @@
     <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="Z1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2075,7 +2083,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3069,7 +3077,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3156,64 +3164,64 @@
         <v>36</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="BH1" s="1" t="s">
         <v>10</v>
@@ -3228,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1503EB05-5C8B-964B-81F7-3D25D9E03BCE}">
   <dimension ref="A1:BX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -3342,7 +3350,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -3429,46 +3437,46 @@
         <v>36</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AQ1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>10</v>
@@ -3477,67 +3485,67 @@
         <v>87</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BE1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BS1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3601,13 +3609,13 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>40</v>
@@ -3616,22 +3624,22 @@
         <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
updating angular version - updated validation tests
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_sample.xlsx
+++ b/src/assets/empty/faang_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yroochun/Projects/dcc-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212E850D-5ED4-694F-BCAD-92DD670CC820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ABCDE5-FF2E-2847-B65B-189C6E530DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34940" yWindow="2080" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
+    <workbookView xWindow="39880" yWindow="8540" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{98093BAA-FAF6-D542-BB9A-98E15CDA65F3}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="140">
   <si>
     <t>Sample Name</t>
   </si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t>Organoid Passage</t>
+  </si>
+  <si>
+    <t>Number Of Frozen Cells</t>
+  </si>
+  <si>
+    <t>Organoid Culture And Passage Protocol</t>
   </si>
 </sst>
 </file>
@@ -1872,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE77F75-4E48-3E4D-BF43-36F736F051D4}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1896,23 +1902,26 @@
     <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1962,36 +1971,45 @@
         <v>91</v>
       </c>
       <c r="Q1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="R1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="9" t="s">
+      <c r="U1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD1" s="9" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>